<commit_message>
added apa script and one result
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -7,14 +7,14 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="最大化发电-无废料-回收钸-允许转化-有红石" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="最大化发电-无废料-回收钸-允许转化-无红石" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="最大化发电-无废料-回收钸-无转化-有红石" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="最大化发电-无废料-回收钸-无转化-无红石" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="最大化发电-无废料-铀钸镄-允许转化-有红石" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="最大化发电-无废料-铀钸镄-允许转化-无红石" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="最大化发电-无废料-铀钸镄-无转化-有红石" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="最大化发电-无废料-铀钸镄-无转化-无红石" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="最大化发电-无废料-钚回收-允许转化-有红石" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="最大化发电-无废料-钚回收-允许转化-无红石" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="最大化发电-无废料-钚回收-无转化-有红石" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="最大化发电-无废料-钚回收-无转化-无红石" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="最大化发电-无废料-铀钚镄-允许转化-有红石" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="最大化发电-无废料-铀钚镄-允许转化-无红石" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="最大化发电-无废料-铀钚镄-无转化-有红石" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="最大化发电-无废料-铀钚镄-无转化-无红石" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="最大化发电-有废料-有红石" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="最大化发电-有废料-无红石" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="最大化点数-降频1%-有红石" sheetId="11" state="visible" r:id="rId11"/>

</xml_diff>